<commit_message>
test detail to xlsx
</commit_message>
<xml_diff>
--- a/ebi-den-su/docs/テスト仕様書.xlsx
+++ b/ebi-den-su/docs/テスト仕様書.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tak/Documents/git/ebi-den-su/ebi-den-su/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3B0807D-C55B-FE4E-90CE-97F4464F970C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BECDA18-4F51-9E4A-9FE4-A6085F0B2C1B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="280" yWindow="3560" windowWidth="28040" windowHeight="17440" xr2:uid="{3771D6DB-D8DF-4A48-8F6E-095AE3805AA1}"/>
+    <workbookView xWindow="620" yWindow="2700" windowWidth="28040" windowHeight="17440" xr2:uid="{3771D6DB-D8DF-4A48-8F6E-095AE3805AA1}"/>
   </bookViews>
   <sheets>
     <sheet name="テストケース" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>クラス</t>
   </si>
@@ -33,9 +33,6 @@
     <t>メソッド</t>
   </si>
   <si>
-    <t>説明</t>
-  </si>
-  <si>
     <t>dense.TestCase1</t>
   </si>
   <si>
@@ -52,6 +49,45 @@
   </si>
   <si>
     <t>テストNO</t>
+  </si>
+  <si>
+    <t>aaaa
+aaaa
+aaaa</t>
+  </si>
+  <si>
+    <t>bbb
+ccc</t>
+  </si>
+  <si>
+    <t>検証項目</t>
+  </si>
+  <si>
+    <t>テスト概要</t>
+  </si>
+  <si>
+    <t>テスト項目</t>
+  </si>
+  <si>
+    <t>テスト</t>
+  </si>
+  <si>
+    <t>テストのテスト１</t>
+  </si>
+  <si>
+    <t>手順</t>
+  </si>
+  <si>
+    <t>1
+2
+3</t>
+  </si>
+  <si>
+    <t>テストのテスト２
+テストのテスト3</t>
+  </si>
+  <si>
+    <t>実施日</t>
   </si>
 </sst>
 </file>
@@ -87,8 +123,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -403,49 +442,81 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D088E3C6-0D47-1540-8498-A5E262BE2318}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="F1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>7</v>
+      <c r="G1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I1" t="s">
+        <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:9" ht="51">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" t="s">
+      <c r="G2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H2" s="1"/>
+    </row>
+    <row r="3" spans="1:9" ht="68">
+      <c r="C3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="B3" t="s">
+      <c r="F3" t="s">
         <v>5</v>
       </c>
-      <c r="C3" t="s">
-        <v>6</v>
-      </c>
+      <c r="G3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H3" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>